<commit_message>
<=15 + new patterns
</commit_message>
<xml_diff>
--- a/resources/xlsx/patterns.xlsx
+++ b/resources/xlsx/patterns.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="45">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -80,6 +80,81 @@
   </si>
   <si>
     <t xml:space="preserve">adjf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">такие arg1, как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">таких arg1, как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">таким arg1, как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg1, таких как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg1, таким как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2,  а также другие arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2,  также как и другие arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2,  и другие arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2,  а также другим arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2,  также как и другим arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2,  и другим arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2,  а также других arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2,  также как и других arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2,  и других arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">виды arg1, как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">типы arg1, как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">формы arg1, как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">разновидности arg1, как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">сорта arg1, как arg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2 — вид arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2 — тип arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2 — форма arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2 — разновидность arg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arg2 — сорт arg1</t>
   </si>
 </sst>
 </file>
@@ -181,19 +256,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.4511627906977"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="12.3953488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1395348837209"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.3953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.8093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.0046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,17 +428,917 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
new ontology+patterns, new ParallelRun, stupid bug fix
</commit_message>
<xml_diff>
--- a/resources/xlsx/patterns.xlsx
+++ b/resources/xlsx/patterns.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="43">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">arg1, таких как arg2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gen</t>
   </si>
   <si>
     <t xml:space="preserve">arg1, таким как arg2</t>
@@ -256,16 +253,13 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.26046511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.3209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="9.26046511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.9813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.26046511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.1860465116279"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,7 +504,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>9</v>
@@ -533,7 +527,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>16</v>
@@ -559,7 +553,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>9</v>
@@ -585,7 +579,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>9</v>
@@ -611,7 +605,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>9</v>
@@ -637,7 +631,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>16</v>
@@ -663,7 +657,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>16</v>
@@ -689,7 +683,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>16</v>
@@ -715,7 +709,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>20</v>
@@ -741,7 +735,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>20</v>
@@ -767,7 +761,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>20</v>
@@ -793,7 +787,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>20</v>
@@ -819,7 +813,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>20</v>
@@ -845,7 +839,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>20</v>
@@ -871,7 +865,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>20</v>
@@ -897,7 +891,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>20</v>
@@ -923,7 +917,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>20</v>
@@ -949,7 +943,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>20</v>
@@ -975,7 +969,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>20</v>
@@ -1001,7 +995,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>20</v>
@@ -1027,7 +1021,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>20</v>
@@ -1053,7 +1047,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>20</v>
@@ -1079,7 +1073,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>20</v>
@@ -1105,7 +1099,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>20</v>
@@ -1131,7 +1125,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>20</v>
@@ -1157,7 +1151,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>20</v>
@@ -1183,7 +1177,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>20</v>
@@ -1209,7 +1203,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>20</v>
@@ -1235,7 +1229,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>20</v>
@@ -1261,7 +1255,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>20</v>
@@ -1287,7 +1281,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>20</v>

</xml_diff>